<commit_message>
added calendar utils, entities and minor ui changes
</commit_message>
<xml_diff>
--- a/TWSCalendar/src/main/resources/CalendarTemp.xlsx
+++ b/TWSCalendar/src/main/resources/CalendarTemp.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13890" windowHeight="2745"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="24">
   <si>
     <t>© www.calendarpedia.com</t>
   </si>
@@ -88,9 +89,6 @@
   </si>
   <si>
     <t>December</t>
-  </si>
-  <si>
-    <t>xxxx Calendar</t>
   </si>
 </sst>
 </file>
@@ -504,28 +502,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -609,6 +586,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -917,7 +915,7 @@
   <dimension ref="B1:AF29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,9 +955,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="45">
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1027,391 +1023,391 @@
       <c r="AF2" s="8"/>
     </row>
     <row r="3" spans="2:32" ht="18.75" thickBot="1">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="9" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="9" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="9" t="s">
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
     </row>
     <row r="4" spans="2:32" ht="18">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="11" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="15" t="s">
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="11" t="s">
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="13"/>
-    </row>
-    <row r="5" spans="2:32" ht="30">
-      <c r="B5" s="18" t="s">
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="45"/>
+    </row>
+    <row r="5" spans="2:32">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="18" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="18" t="s">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="W5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="43" t="s">
+      <c r="X5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="18" t="s">
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="19" t="s">
+      <c r="AA5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="19" t="s">
+      <c r="AB5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" s="19" t="s">
+      <c r="AC5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AD5" s="19" t="s">
+      <c r="AD5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AE5" s="19" t="s">
+      <c r="AE5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AF5" s="20" t="s">
+      <c r="AF5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:32" ht="15.75">
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="25"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="18"/>
     </row>
     <row r="7" spans="2:32" ht="15.75">
-      <c r="B7" s="26"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="25"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="18"/>
     </row>
     <row r="8" spans="2:32" ht="15.75">
-      <c r="B8" s="26"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="25"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="18"/>
     </row>
     <row r="9" spans="2:32" ht="15.75">
-      <c r="B9" s="26"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="25"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="18"/>
     </row>
     <row r="10" spans="2:32" ht="15.75">
-      <c r="B10" s="26"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="23"/>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="25"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10" s="16"/>
+      <c r="AF10" s="18"/>
     </row>
     <row r="11" spans="2:32" ht="16.5" thickBot="1">
-      <c r="B11" s="38"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="37"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="37"/>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="37"/>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="37"/>
-      <c r="AD11" s="37"/>
-      <c r="AE11" s="37"/>
-      <c r="AF11" s="41"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="34"/>
     </row>
     <row r="12" spans="2:32" ht="18.75" thickBot="1">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1419,342 +1415,342 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="31"/>
-      <c r="AB12" s="31"/>
-      <c r="AC12" s="31"/>
-      <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="32"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="25"/>
     </row>
     <row r="13" spans="2:32" ht="18">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="15" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="15" t="s">
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="11" t="s">
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="13"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="44"/>
+      <c r="AD13" s="44"/>
+      <c r="AE13" s="44"/>
+      <c r="AF13" s="45"/>
     </row>
     <row r="14" spans="2:32">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="18" t="s">
+      <c r="I14" s="26"/>
+      <c r="J14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="20" t="s">
+      <c r="P14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="18" t="s">
+      <c r="Q14" s="26"/>
+      <c r="R14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="19" t="s">
+      <c r="S14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="T14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="U14" s="19" t="s">
+      <c r="U14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="V14" s="19" t="s">
+      <c r="V14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="W14" s="19" t="s">
+      <c r="W14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="20" t="s">
+      <c r="X14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="18" t="s">
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AA14" s="19" t="s">
+      <c r="AA14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AB14" s="19" t="s">
+      <c r="AB14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AC14" s="19" t="s">
+      <c r="AC14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AD14" s="19" t="s">
+      <c r="AD14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AE14" s="19" t="s">
+      <c r="AE14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AF14" s="20" t="s">
+      <c r="AF14" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:32" ht="15.75">
-      <c r="B15" s="26"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="25"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="25"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="18"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="25"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="18"/>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="25"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="18"/>
     </row>
     <row r="16" spans="2:32" ht="15.75">
-      <c r="B16" s="26"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="25"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="25"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="18"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="25"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="18"/>
       <c r="Y16" s="3"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="25"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="18"/>
     </row>
     <row r="17" spans="2:32" ht="15.75">
-      <c r="B17" s="26"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="25"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="18"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="25"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="18"/>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="25"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="18"/>
     </row>
     <row r="18" spans="2:32" ht="15.75">
-      <c r="B18" s="26"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="35"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="25"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="3"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="25"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="18"/>
       <c r="Y18" s="3"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="25"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="18"/>
     </row>
     <row r="19" spans="2:32" ht="15.75">
-      <c r="B19" s="26"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="40"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="33"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="35"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="28"/>
       <c r="Q19" s="3"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="35"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="28"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="35"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="16"/>
+      <c r="AC19" s="16"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="28"/>
     </row>
     <row r="20" spans="2:32" ht="16.5" thickBot="1">
-      <c r="B20" s="38"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="39"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="28"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="21"/>
       <c r="Q20" s="3"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="28"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="21"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="37"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="37"/>
-      <c r="AD20" s="37"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="39"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="30"/>
+      <c r="AB20" s="30"/>
+      <c r="AC20" s="30"/>
+      <c r="AD20" s="30"/>
+      <c r="AE20" s="30"/>
+      <c r="AF20" s="32"/>
     </row>
     <row r="21" spans="2:32" ht="15.75" thickBot="1">
       <c r="B21" s="3"/>
@@ -1790,348 +1786,348 @@
       <c r="AF21" s="3"/>
     </row>
     <row r="22" spans="2:32" ht="18">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="17"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="13"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="15" t="s">
+      <c r="R22" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="17"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="42"/>
       <c r="Y22" s="3"/>
-      <c r="Z22" s="11" t="s">
+      <c r="Z22" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
-      <c r="AE22" s="12"/>
-      <c r="AF22" s="13"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="44"/>
+      <c r="AD22" s="44"/>
+      <c r="AE22" s="44"/>
+      <c r="AF22" s="45"/>
     </row>
     <row r="23" spans="2:32">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="13" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O23" s="19" t="s">
+      <c r="O23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P23" s="20" t="s">
+      <c r="P23" s="13" t="s">
         <v>15</v>
       </c>
       <c r="Q23" s="3"/>
-      <c r="R23" s="18" t="s">
+      <c r="R23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S23" s="19" t="s">
+      <c r="S23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="T23" s="19" t="s">
+      <c r="T23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="U23" s="19" t="s">
+      <c r="U23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="V23" s="19" t="s">
+      <c r="V23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="W23" s="19" t="s">
+      <c r="W23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="X23" s="20" t="s">
+      <c r="X23" s="13" t="s">
         <v>15</v>
       </c>
       <c r="Y23" s="3"/>
-      <c r="Z23" s="18" t="s">
+      <c r="Z23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AA23" s="19" t="s">
+      <c r="AA23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AB23" s="19" t="s">
+      <c r="AB23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AC23" s="19" t="s">
+      <c r="AC23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AD23" s="19" t="s">
+      <c r="AD23" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AE23" s="19" t="s">
+      <c r="AE23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AF23" s="20" t="s">
+      <c r="AF23" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:32" ht="15.75">
-      <c r="B24" s="26"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="25"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="18"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="25"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="18"/>
       <c r="Q24" s="3"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="25"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="18"/>
       <c r="Y24" s="3"/>
-      <c r="Z24" s="22"/>
-      <c r="AA24" s="23"/>
-      <c r="AB24" s="23"/>
-      <c r="AC24" s="23"/>
-      <c r="AD24" s="23"/>
-      <c r="AE24" s="23"/>
-      <c r="AF24" s="25"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="16"/>
+      <c r="AB24" s="16"/>
+      <c r="AC24" s="16"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="18"/>
     </row>
     <row r="25" spans="2:32" ht="15.75">
-      <c r="B25" s="26"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="25"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="18"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="25"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="18"/>
       <c r="Q25" s="3"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="25"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="18"/>
       <c r="Y25" s="3"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="23"/>
-      <c r="AB25" s="23"/>
-      <c r="AC25" s="23"/>
-      <c r="AD25" s="23"/>
-      <c r="AE25" s="23"/>
-      <c r="AF25" s="25"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="16"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="16"/>
+      <c r="AF25" s="18"/>
     </row>
     <row r="26" spans="2:32" ht="15.75">
-      <c r="B26" s="26"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="25"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="25"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="18"/>
       <c r="Q26" s="3"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="25"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="18"/>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="23"/>
-      <c r="AB26" s="23"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="23"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="25"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="16"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="18"/>
     </row>
     <row r="27" spans="2:32" ht="15.75">
-      <c r="B27" s="26"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="25"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="18"/>
       <c r="Q27" s="3"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="25"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="18"/>
       <c r="Y27" s="3"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="23"/>
-      <c r="AB27" s="23"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="23"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="25"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="16"/>
+      <c r="AD27" s="16"/>
+      <c r="AE27" s="17"/>
+      <c r="AF27" s="18"/>
     </row>
     <row r="28" spans="2:32" ht="15.75">
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="35"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="35"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="28"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="35"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="28"/>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="23"/>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="23"/>
-      <c r="AD28" s="23"/>
-      <c r="AE28" s="23"/>
-      <c r="AF28" s="35"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="16"/>
+      <c r="AB28" s="16"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="28"/>
     </row>
     <row r="29" spans="2:32" ht="16.5" thickBot="1">
-      <c r="B29" s="46"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="39"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="39"/>
-      <c r="R29" s="38"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="37"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="39"/>
-      <c r="Z29" s="38"/>
-      <c r="AA29" s="37"/>
-      <c r="AB29" s="37"/>
-      <c r="AC29" s="37"/>
-      <c r="AD29" s="37"/>
-      <c r="AE29" s="37"/>
-      <c r="AF29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="32"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="32"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="32"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="30"/>
+      <c r="AB29" s="30"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="30"/>
+      <c r="AE29" s="30"/>
+      <c r="AF29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R3:X3"/>
+    <mergeCell ref="Z3:AF3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J3:P3"/>
     <mergeCell ref="R13:X13"/>
     <mergeCell ref="Z13:AF13"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="J22:P22"/>
     <mergeCell ref="R22:X22"/>
     <mergeCell ref="Z22:AF22"/>
-    <mergeCell ref="R3:X3"/>
-    <mergeCell ref="Z3:AF3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="Z4:AF4"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="J13:P13"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="J3:P3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD1" r:id="rId1" display="© www.calendarpedia.co.uk"/>

</xml_diff>